<commit_message>
cost functions and weights check fix
</commit_message>
<xml_diff>
--- a/lecturer_availability.xlsx
+++ b/lecturer_availability.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Result" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Result" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1188,7 +1188,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C24" s="3" t="inlineStr">
+      <c r="C24" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1220,7 +1220,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C25" s="3" t="inlineStr">
+      <c r="C25" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1252,7 +1252,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C26" s="3" t="inlineStr">
+      <c r="C26" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1284,7 +1284,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C27" s="3" t="inlineStr">
+      <c r="C27" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1316,7 +1316,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C28" s="3" t="inlineStr">
+      <c r="C28" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1348,7 +1348,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C29" s="3" t="inlineStr">
+      <c r="C29" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1380,7 +1380,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C30" s="3" t="inlineStr">
+      <c r="C30" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1412,7 +1412,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C31" s="3" t="inlineStr">
+      <c r="C31" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1444,7 +1444,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C32" s="3" t="inlineStr">
+      <c r="C32" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1476,7 +1476,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C33" s="3" t="inlineStr">
+      <c r="C33" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1508,7 +1508,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C34" s="3" t="inlineStr">
+      <c r="C34" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1540,7 +1540,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C35" s="3" t="inlineStr">
+      <c r="C35" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1572,7 +1572,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C36" s="3" t="inlineStr">
+      <c r="C36" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1604,7 +1604,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C37" s="3" t="inlineStr">
+      <c r="C37" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1636,7 +1636,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C38" s="3" t="inlineStr">
+      <c r="C38" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1668,7 +1668,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C39" s="3" t="inlineStr">
+      <c r="C39" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1700,7 +1700,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C40" s="3" t="inlineStr">
+      <c r="C40" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1732,7 +1732,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C41" s="3" t="inlineStr">
+      <c r="C41" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1764,7 +1764,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C42" s="3" t="inlineStr">
+      <c r="C42" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1796,7 +1796,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C43" s="3" t="inlineStr">
+      <c r="C43" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1828,7 +1828,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C44" s="3" t="inlineStr">
+      <c r="C44" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1860,7 +1860,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C45" s="3" t="inlineStr">
+      <c r="C45" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1875,7 +1875,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F45" s="4" t="inlineStr">
+      <c r="F45" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1892,7 +1892,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C46" s="3" t="inlineStr">
+      <c r="C46" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1907,7 +1907,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F46" s="4" t="inlineStr">
+      <c r="F46" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1924,7 +1924,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C47" s="3" t="inlineStr">
+      <c r="C47" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1939,7 +1939,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F47" s="4" t="inlineStr">
+      <c r="F47" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1956,7 +1956,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C48" s="3" t="inlineStr">
+      <c r="C48" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1971,7 +1971,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F48" s="4" t="inlineStr">
+      <c r="F48" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -1988,7 +1988,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C49" s="3" t="inlineStr">
+      <c r="C49" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2003,7 +2003,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F49" s="4" t="inlineStr">
+      <c r="F49" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2035,7 +2035,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F50" s="4" t="inlineStr">
+      <c r="F50" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2067,7 +2067,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F51" s="4" t="inlineStr">
+      <c r="F51" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2099,7 +2099,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F52" s="4" t="inlineStr">
+      <c r="F52" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2131,7 +2131,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F53" s="4" t="inlineStr">
+      <c r="F53" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2163,7 +2163,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F54" s="4" t="inlineStr">
+      <c r="F54" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2195,7 +2195,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F55" s="4" t="inlineStr">
+      <c r="F55" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2227,7 +2227,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F56" s="4" t="inlineStr">
+      <c r="F56" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2259,7 +2259,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F57" s="4" t="inlineStr">
+      <c r="F57" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2291,7 +2291,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F58" s="4" t="inlineStr">
+      <c r="F58" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2323,7 +2323,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F59" s="4" t="inlineStr">
+      <c r="F59" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2355,7 +2355,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F60" s="4" t="inlineStr">
+      <c r="F60" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2387,7 +2387,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F61" s="4" t="inlineStr">
+      <c r="F61" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2419,7 +2419,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F62" s="4" t="inlineStr">
+      <c r="F62" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2451,7 +2451,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F63" s="4" t="inlineStr">
+      <c r="F63" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2483,7 +2483,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F64" s="4" t="inlineStr">
+      <c r="F64" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2515,7 +2515,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F65" s="4" t="inlineStr">
+      <c r="F65" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2527,7 +2527,7 @@
           <t>13:15</t>
         </is>
       </c>
-      <c r="B66" s="3" t="inlineStr">
+      <c r="B66" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2547,7 +2547,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F66" s="4" t="inlineStr">
+      <c r="F66" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2559,7 +2559,7 @@
           <t>13:20</t>
         </is>
       </c>
-      <c r="B67" s="3" t="inlineStr">
+      <c r="B67" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2579,7 +2579,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F67" s="4" t="inlineStr">
+      <c r="F67" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2591,7 +2591,7 @@
           <t>13:25</t>
         </is>
       </c>
-      <c r="B68" s="3" t="inlineStr">
+      <c r="B68" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2611,7 +2611,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F68" s="4" t="inlineStr">
+      <c r="F68" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2623,7 +2623,7 @@
           <t>13:30</t>
         </is>
       </c>
-      <c r="B69" s="3" t="inlineStr">
+      <c r="B69" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2643,7 +2643,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F69" s="4" t="inlineStr">
+      <c r="F69" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2655,7 +2655,7 @@
           <t>13:35</t>
         </is>
       </c>
-      <c r="B70" s="3" t="inlineStr">
+      <c r="B70" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2675,7 +2675,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F70" s="4" t="inlineStr">
+      <c r="F70" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2687,7 +2687,7 @@
           <t>13:40</t>
         </is>
       </c>
-      <c r="B71" s="3" t="inlineStr">
+      <c r="B71" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2719,7 +2719,7 @@
           <t>13:45</t>
         </is>
       </c>
-      <c r="B72" s="3" t="inlineStr">
+      <c r="B72" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2751,7 +2751,7 @@
           <t>13:50</t>
         </is>
       </c>
-      <c r="B73" s="3" t="inlineStr">
+      <c r="B73" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2783,7 +2783,7 @@
           <t>13:55</t>
         </is>
       </c>
-      <c r="B74" s="3" t="inlineStr">
+      <c r="B74" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2815,7 +2815,7 @@
           <t>14:00</t>
         </is>
       </c>
-      <c r="B75" s="3" t="inlineStr">
+      <c r="B75" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2847,7 +2847,7 @@
           <t>14:05</t>
         </is>
       </c>
-      <c r="B76" s="3" t="inlineStr">
+      <c r="B76" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2879,7 +2879,7 @@
           <t>14:10</t>
         </is>
       </c>
-      <c r="B77" s="3" t="inlineStr">
+      <c r="B77" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2911,7 +2911,7 @@
           <t>14:15</t>
         </is>
       </c>
-      <c r="B78" s="3" t="inlineStr">
+      <c r="B78" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2943,7 +2943,7 @@
           <t>14:20</t>
         </is>
       </c>
-      <c r="B79" s="3" t="inlineStr">
+      <c r="B79" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -2975,7 +2975,7 @@
           <t>14:25</t>
         </is>
       </c>
-      <c r="B80" s="3" t="inlineStr">
+      <c r="B80" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3007,7 +3007,7 @@
           <t>14:30</t>
         </is>
       </c>
-      <c r="B81" s="3" t="inlineStr">
+      <c r="B81" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3039,7 +3039,7 @@
           <t>14:35</t>
         </is>
       </c>
-      <c r="B82" s="3" t="inlineStr">
+      <c r="B82" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3071,7 +3071,7 @@
           <t>14:40</t>
         </is>
       </c>
-      <c r="B83" s="3" t="inlineStr">
+      <c r="B83" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3103,7 +3103,7 @@
           <t>14:45</t>
         </is>
       </c>
-      <c r="B84" s="3" t="inlineStr">
+      <c r="B84" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3135,7 +3135,7 @@
           <t>14:50</t>
         </is>
       </c>
-      <c r="B85" s="3" t="inlineStr">
+      <c r="B85" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3167,7 +3167,7 @@
           <t>14:55</t>
         </is>
       </c>
-      <c r="B86" s="3" t="inlineStr">
+      <c r="B86" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3199,7 +3199,7 @@
           <t>15:00</t>
         </is>
       </c>
-      <c r="B87" s="3" t="inlineStr">
+      <c r="B87" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3231,7 +3231,7 @@
           <t>15:05</t>
         </is>
       </c>
-      <c r="B88" s="3" t="inlineStr">
+      <c r="B88" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3263,7 +3263,7 @@
           <t>15:10</t>
         </is>
       </c>
-      <c r="B89" s="3" t="inlineStr">
+      <c r="B89" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3295,7 +3295,7 @@
           <t>15:15</t>
         </is>
       </c>
-      <c r="B90" s="3" t="inlineStr">
+      <c r="B90" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3327,7 +3327,7 @@
           <t>15:20</t>
         </is>
       </c>
-      <c r="B91" s="3" t="inlineStr">
+      <c r="B91" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3785,7 +3785,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D105" s="4" t="inlineStr">
+      <c r="D105" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3817,7 +3817,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D106" s="4" t="inlineStr">
+      <c r="D106" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3849,7 +3849,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D107" s="4" t="inlineStr">
+      <c r="D107" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3881,7 +3881,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D108" s="4" t="inlineStr">
+      <c r="D108" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3913,7 +3913,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D109" s="4" t="inlineStr">
+      <c r="D109" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3945,7 +3945,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D110" s="4" t="inlineStr">
+      <c r="D110" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -3977,7 +3977,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D111" s="4" t="inlineStr">
+      <c r="D111" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4009,7 +4009,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D112" s="4" t="inlineStr">
+      <c r="D112" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4041,7 +4041,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D113" s="4" t="inlineStr">
+      <c r="D113" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4073,7 +4073,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D114" s="4" t="inlineStr">
+      <c r="D114" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4105,7 +4105,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D115" s="4" t="inlineStr">
+      <c r="D115" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4137,7 +4137,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D116" s="4" t="inlineStr">
+      <c r="D116" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4169,7 +4169,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D117" s="4" t="inlineStr">
+      <c r="D117" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4201,7 +4201,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D118" s="4" t="inlineStr">
+      <c r="D118" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4233,7 +4233,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D119" s="4" t="inlineStr">
+      <c r="D119" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4265,7 +4265,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D120" s="4" t="inlineStr">
+      <c r="D120" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4297,7 +4297,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D121" s="4" t="inlineStr">
+      <c r="D121" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4329,7 +4329,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D122" s="4" t="inlineStr">
+      <c r="D122" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4361,7 +4361,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D123" s="4" t="inlineStr">
+      <c r="D123" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4393,7 +4393,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D124" s="4" t="inlineStr">
+      <c r="D124" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4425,7 +4425,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D125" s="4" t="inlineStr">
+      <c r="D125" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4457,7 +4457,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D126" s="4" t="inlineStr">
+      <c r="D126" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4489,7 +4489,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D127" s="4" t="inlineStr">
+      <c r="D127" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4521,7 +4521,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D128" s="4" t="inlineStr">
+      <c r="D128" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4553,7 +4553,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D129" s="4" t="inlineStr">
+      <c r="D129" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
@@ -4585,7 +4585,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D130" s="4" t="inlineStr">
+      <c r="D130" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>

</xml_diff>